<commit_message>
Ajustando função criação do pedido a cada seleção
</commit_message>
<xml_diff>
--- a/mercadoria.xlsx
+++ b/mercadoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos_Phayton\Primeiro_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A045EA28-B2E8-4E27-BDCD-FCB5D11B7FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC61E085-F48C-4D7D-9E77-E1EC8F270502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DAC61F51-090E-4E48-8FA2-8D704C875542}"/>
   </bookViews>
@@ -44,18 +44,6 @@
     <t>desc_produto</t>
   </si>
   <si>
-    <t>quantidade1</t>
-  </si>
-  <si>
-    <t>quantidade2</t>
-  </si>
-  <si>
-    <t>quantidade3</t>
-  </si>
-  <si>
-    <t>quantidade4</t>
-  </si>
-  <si>
     <t>pedido</t>
   </si>
   <si>
@@ -156,6 +144,18 @@
   </si>
   <si>
     <t>FLOR LIRIOS VARIADOS PT 15</t>
+  </si>
+  <si>
+    <t>minimo</t>
+  </si>
+  <si>
+    <t>qtd2</t>
+  </si>
+  <si>
+    <t>qtd4</t>
+  </si>
+  <si>
+    <t>qtd3</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -604,19 +604,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75">
@@ -624,7 +624,7 @@
         <v>1097064</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5">
         <v>15</v>
@@ -645,7 +645,7 @@
         <v>1099663</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5">
         <v>15</v>
@@ -666,7 +666,7 @@
         <v>1080071</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="5">
         <v>12</v>
@@ -687,7 +687,7 @@
         <v>1097068</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="5">
         <v>12</v>
@@ -708,7 +708,7 @@
         <v>1080082</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="5">
         <v>12</v>
@@ -729,7 +729,7 @@
         <v>1159663</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" s="5">
         <v>12</v>
@@ -750,7 +750,7 @@
         <v>1129914</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5">
         <v>15</v>
@@ -771,7 +771,7 @@
         <v>1080076</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5">
         <v>10</v>
@@ -792,7 +792,7 @@
         <v>1080077</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C10" s="5">
         <v>8</v>
@@ -813,7 +813,7 @@
         <v>1097085</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C11" s="5">
         <v>3</v>
@@ -834,7 +834,7 @@
         <v>1134845</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C12" s="5">
         <v>12</v>
@@ -855,7 +855,7 @@
         <v>1097067</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C13" s="5">
         <v>15</v>
@@ -876,7 +876,7 @@
         <v>1099659</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C14" s="5">
         <v>15</v>
@@ -897,7 +897,7 @@
         <v>1080073</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5">
         <v>12</v>
@@ -918,7 +918,7 @@
         <v>1097074</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C16" s="5">
         <v>12</v>
@@ -939,7 +939,7 @@
         <v>1097082</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5">
         <v>12</v>
@@ -960,7 +960,7 @@
         <v>1151765</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C18" s="5">
         <v>12</v>
@@ -981,7 +981,7 @@
         <v>1081854</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C19" s="5">
         <v>8</v>
@@ -1002,7 +1002,7 @@
         <v>1118534</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C20" s="5">
         <v>3</v>
@@ -1023,7 +1023,7 @@
         <v>1134669</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C21" s="5">
         <v>12</v>
@@ -1044,7 +1044,7 @@
         <v>1136712</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C22" s="5">
         <v>15</v>
@@ -1065,7 +1065,7 @@
         <v>1134848</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C23" s="5">
         <v>15</v>
@@ -1086,7 +1086,7 @@
         <v>1097061</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C24" s="5">
         <v>12</v>
@@ -1107,7 +1107,7 @@
         <v>1097081</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C25" s="5">
         <v>12</v>
@@ -1128,7 +1128,7 @@
         <v>1122507</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>12</v>
@@ -1149,7 +1149,7 @@
         <v>1099654</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5">
         <v>12</v>
@@ -1170,7 +1170,7 @@
         <v>1102151</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C28" s="5">
         <v>10</v>
@@ -1191,7 +1191,7 @@
         <v>1099662</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C29" s="5">
         <v>8</v>
@@ -1212,7 +1212,7 @@
         <v>1134843</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C30" s="5">
         <v>3</v>
@@ -1233,7 +1233,7 @@
         <v>1080083</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C31" s="5">
         <v>12</v>
@@ -1254,7 +1254,7 @@
         <v>1152107</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C32" s="5">
         <v>15</v>
@@ -1275,7 +1275,7 @@
         <v>1134668</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C33" s="5">
         <v>15</v>
@@ -1296,7 +1296,7 @@
         <v>1097072</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C34" s="5">
         <v>12</v>

</xml_diff>

<commit_message>
Alterado a forma de entrada de dados para quantidade
</commit_message>
<xml_diff>
--- a/mercadoria.xlsx
+++ b/mercadoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos_Phayton\Primeiro_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC61E085-F48C-4D7D-9E77-E1EC8F270502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D378A039-25F7-4FFF-BC2C-3143821460EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DAC61F51-090E-4E48-8FA2-8D704C875542}"/>
   </bookViews>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>cod_produto</t>
   </si>
   <si>
     <t>desc_produto</t>
-  </si>
-  <si>
-    <t>pedido</t>
   </si>
   <si>
     <t>PLANTA SUCULENTA PT 06</t>
@@ -582,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9DE960-2683-4898-8AD4-BC5936F3A2B4}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -593,10 +590,9 @@
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,27 +600,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75">
+    </row>
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="3">
         <v>1097064</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5">
         <v>15</v>
@@ -638,14 +631,13 @@
       <c r="F2" s="5">
         <v>90</v>
       </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75">
+    </row>
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" s="3">
         <v>1099663</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="5">
         <v>15</v>
@@ -659,14 +651,13 @@
       <c r="F3" s="5">
         <v>90</v>
       </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75">
+    </row>
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="3">
         <v>1080071</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5">
         <v>12</v>
@@ -680,14 +671,13 @@
       <c r="F4" s="5">
         <v>72</v>
       </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75">
+    </row>
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="3">
         <v>1097068</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="5">
         <v>12</v>
@@ -701,14 +691,13 @@
       <c r="F5" s="5">
         <v>72</v>
       </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75">
+    </row>
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="3">
         <v>1080082</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="5">
         <v>12</v>
@@ -722,14 +711,13 @@
       <c r="F6" s="5">
         <v>72</v>
       </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75">
+    </row>
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="3">
         <v>1159663</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5">
         <v>12</v>
@@ -743,14 +731,13 @@
       <c r="F7" s="5">
         <v>72</v>
       </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75">
+    </row>
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="3">
         <v>1129914</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="5">
         <v>15</v>
@@ -764,14 +751,13 @@
       <c r="F8" s="5">
         <v>90</v>
       </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75">
+    </row>
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" s="3">
         <v>1080076</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="5">
         <v>10</v>
@@ -785,14 +771,13 @@
       <c r="F9" s="5">
         <v>60</v>
       </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75">
+    </row>
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" s="3">
         <v>1080077</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5">
         <v>8</v>
@@ -806,14 +791,13 @@
       <c r="F10" s="5">
         <v>64</v>
       </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75">
+    </row>
+    <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="3">
         <v>1097085</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="5">
         <v>3</v>
@@ -827,14 +811,13 @@
       <c r="F11" s="5">
         <v>24</v>
       </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75">
+    </row>
+    <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="3">
         <v>1134845</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="5">
         <v>12</v>
@@ -848,14 +831,13 @@
       <c r="F12" s="5">
         <v>72</v>
       </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75">
+    </row>
+    <row r="13" spans="1:6" ht="15.75">
       <c r="A13" s="3">
         <v>1097067</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="5">
         <v>15</v>
@@ -869,14 +851,13 @@
       <c r="F13" s="5">
         <v>90</v>
       </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75">
+    </row>
+    <row r="14" spans="1:6" ht="15.75">
       <c r="A14" s="3">
         <v>1099659</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5">
         <v>15</v>
@@ -890,14 +871,13 @@
       <c r="F14" s="5">
         <v>90</v>
       </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75">
+    </row>
+    <row r="15" spans="1:6" ht="15.75">
       <c r="A15" s="3">
         <v>1080073</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="5">
         <v>12</v>
@@ -911,14 +891,13 @@
       <c r="F15" s="5">
         <v>72</v>
       </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75">
+    </row>
+    <row r="16" spans="1:6" ht="15.75">
       <c r="A16" s="3">
         <v>1097074</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="5">
         <v>12</v>
@@ -932,14 +911,13 @@
       <c r="F16" s="5">
         <v>72</v>
       </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75">
+    </row>
+    <row r="17" spans="1:6" ht="15.75">
       <c r="A17" s="3">
         <v>1097082</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="5">
         <v>12</v>
@@ -953,14 +931,13 @@
       <c r="F17" s="5">
         <v>72</v>
       </c>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75">
+    </row>
+    <row r="18" spans="1:6" ht="15.75">
       <c r="A18" s="3">
         <v>1151765</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5">
         <v>12</v>
@@ -974,14 +951,13 @@
       <c r="F18" s="5">
         <v>72</v>
       </c>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75">
+    </row>
+    <row r="19" spans="1:6" ht="15.75">
       <c r="A19" s="3">
         <v>1081854</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="5">
         <v>8</v>
@@ -995,14 +971,13 @@
       <c r="F19" s="5">
         <v>64</v>
       </c>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75">
+    </row>
+    <row r="20" spans="1:6" ht="15.75">
       <c r="A20" s="3">
         <v>1118534</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5">
         <v>3</v>
@@ -1016,14 +991,13 @@
       <c r="F20" s="5">
         <v>24</v>
       </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75">
+    </row>
+    <row r="21" spans="1:6" ht="15.75">
       <c r="A21" s="3">
         <v>1134669</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="5">
         <v>12</v>
@@ -1037,14 +1011,13 @@
       <c r="F21" s="5">
         <v>72</v>
       </c>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75">
+    </row>
+    <row r="22" spans="1:6" ht="15.75">
       <c r="A22" s="3">
         <v>1136712</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="5">
         <v>15</v>
@@ -1058,14 +1031,13 @@
       <c r="F22" s="5">
         <v>90</v>
       </c>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75">
+    </row>
+    <row r="23" spans="1:6" ht="15.75">
       <c r="A23" s="3">
         <v>1134848</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="5">
         <v>15</v>
@@ -1079,14 +1051,13 @@
       <c r="F23" s="5">
         <v>90</v>
       </c>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75">
+    </row>
+    <row r="24" spans="1:6" ht="15.75">
       <c r="A24" s="3">
         <v>1097061</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="5">
         <v>12</v>
@@ -1100,14 +1071,13 @@
       <c r="F24" s="5">
         <v>72</v>
       </c>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75">
+    </row>
+    <row r="25" spans="1:6" ht="15.75">
       <c r="A25" s="3">
         <v>1097081</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="5">
         <v>12</v>
@@ -1121,14 +1091,13 @@
       <c r="F25" s="5">
         <v>72</v>
       </c>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75">
+    </row>
+    <row r="26" spans="1:6" ht="15.75">
       <c r="A26" s="3">
         <v>1122507</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5">
         <v>12</v>
@@ -1142,14 +1111,13 @@
       <c r="F26" s="5">
         <v>72</v>
       </c>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75">
+    </row>
+    <row r="27" spans="1:6" ht="15.75">
       <c r="A27" s="3">
         <v>1099654</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5">
         <v>12</v>
@@ -1163,14 +1131,13 @@
       <c r="F27" s="5">
         <v>72</v>
       </c>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75">
+    </row>
+    <row r="28" spans="1:6" ht="15.75">
       <c r="A28" s="3">
         <v>1102151</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="5">
         <v>10</v>
@@ -1184,14 +1151,13 @@
       <c r="F28" s="5">
         <v>60</v>
       </c>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75">
+    </row>
+    <row r="29" spans="1:6" ht="15.75">
       <c r="A29" s="3">
         <v>1099662</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="5">
         <v>8</v>
@@ -1205,14 +1171,13 @@
       <c r="F29" s="5">
         <v>64</v>
       </c>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75">
+    </row>
+    <row r="30" spans="1:6" ht="15.75">
       <c r="A30" s="3">
         <v>1134843</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="5">
         <v>3</v>
@@ -1226,14 +1191,13 @@
       <c r="F30" s="5">
         <v>24</v>
       </c>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75">
+    </row>
+    <row r="31" spans="1:6" ht="15.75">
       <c r="A31" s="3">
         <v>1080083</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="5">
         <v>12</v>
@@ -1247,14 +1211,13 @@
       <c r="F31" s="5">
         <v>72</v>
       </c>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75">
+    </row>
+    <row r="32" spans="1:6" ht="15.75">
       <c r="A32" s="3">
         <v>1152107</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="5">
         <v>15</v>
@@ -1268,14 +1231,13 @@
       <c r="F32" s="5">
         <v>90</v>
       </c>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75">
+    </row>
+    <row r="33" spans="1:6" ht="15.75">
       <c r="A33" s="3">
         <v>1134668</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="5">
         <v>15</v>
@@ -1289,14 +1251,13 @@
       <c r="F33" s="5">
         <v>90</v>
       </c>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75">
+    </row>
+    <row r="34" spans="1:6" ht="15.75">
       <c r="A34" s="3">
         <v>1097072</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="5">
         <v>12</v>
@@ -1310,7 +1271,6 @@
       <c r="F34" s="5">
         <v>72</v>
       </c>
-      <c r="G34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
incluindo conexão de base de dados
</commit_message>
<xml_diff>
--- a/mercadoria.xlsx
+++ b/mercadoria.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos_Phayton\Primeiro_Dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos_Phayton\Primeiro_Projeto_Pedidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E192FE3-005F-4BFC-9AC0-AA915307B8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47C982B-CF4D-4B96-86D6-6968DE11F731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DAC61F51-090E-4E48-8FA2-8D704C875542}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{DAC61F51-090E-4E48-8FA2-8D704C875542}"/>
   </bookViews>
   <sheets>
-    <sheet name="pedido" sheetId="1" r:id="rId1"/>
+    <sheet name="Descricao" sheetId="1" r:id="rId1"/>
+    <sheet name="Loja" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -581,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9DE960-2683-4898-8AD4-BC5936F3A2B4}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1275,4 +1276,18 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5E86BA-4545-4091-B845-A9E9CE6DCE14}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implementando a visualização de imagem
</commit_message>
<xml_diff>
--- a/mercadoria.xlsx
+++ b/mercadoria.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos_Phayton\Primeiro_Projeto_Pedidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47C982B-CF4D-4B96-86D6-6968DE11F731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EF2FA5-9422-499D-BEE6-BD93B17710ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{DAC61F51-090E-4E48-8FA2-8D704C875542}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DAC61F51-090E-4E48-8FA2-8D704C875542}"/>
   </bookViews>
   <sheets>
     <sheet name="Descricao" sheetId="1" r:id="rId1"/>
-    <sheet name="Loja" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>cod_produto</t>
   </si>
@@ -142,18 +141,6 @@
   </si>
   <si>
     <t>FLOR LIRIOS VARIADOS PT 15</t>
-  </si>
-  <si>
-    <t>minimo</t>
-  </si>
-  <si>
-    <t>qtd2</t>
-  </si>
-  <si>
-    <t>qtd4</t>
-  </si>
-  <si>
-    <t>qtd3</t>
   </si>
 </sst>
 </file>
@@ -187,7 +174,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +190,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2F0D9"/>
+        <bgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
@@ -248,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -262,8 +255,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -284,9 +280,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -324,7 +320,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -430,7 +426,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -572,7 +568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -580,714 +576,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9DE960-2683-4898-8AD4-BC5936F3A2B4}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75">
+    </row>
+    <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="3">
         <v>1097064</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5">
-        <v>15</v>
-      </c>
-      <c r="D2" s="5">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5">
-        <v>45</v>
-      </c>
-      <c r="F2" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75">
+    </row>
+    <row r="3" spans="1:2" ht="15.75">
       <c r="A3" s="3">
         <v>1099663</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5">
-        <v>30</v>
-      </c>
-      <c r="E3" s="5">
-        <v>45</v>
-      </c>
-      <c r="F3" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75">
+    </row>
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="3">
         <v>1080071</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5">
-        <v>24</v>
-      </c>
-      <c r="E4" s="5">
-        <v>36</v>
-      </c>
-      <c r="F4" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75">
+    </row>
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="3">
         <v>1097068</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5">
-        <v>24</v>
-      </c>
-      <c r="E5" s="5">
-        <v>36</v>
-      </c>
-      <c r="F5" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75">
+    </row>
+    <row r="6" spans="1:2" ht="15.75">
       <c r="A6" s="3">
         <v>1080082</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5">
-        <v>24</v>
-      </c>
-      <c r="E6" s="5">
-        <v>36</v>
-      </c>
-      <c r="F6" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75">
+    </row>
+    <row r="7" spans="1:2" ht="15.75">
       <c r="A7" s="3">
         <v>1159663</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5">
-        <v>24</v>
-      </c>
-      <c r="E7" s="5">
-        <v>36</v>
-      </c>
-      <c r="F7" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75">
+    </row>
+    <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="3">
         <v>1129914</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="5">
-        <v>15</v>
-      </c>
-      <c r="D8" s="5">
-        <v>30</v>
-      </c>
-      <c r="E8" s="5">
-        <v>45</v>
-      </c>
-      <c r="F8" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75">
-      <c r="A9" s="3">
+    </row>
+    <row r="9" spans="1:2" ht="15.75">
+      <c r="A9" s="5">
         <v>1080076</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="5">
-        <v>10</v>
-      </c>
-      <c r="D9" s="5">
-        <v>20</v>
-      </c>
-      <c r="E9" s="5">
-        <v>30</v>
-      </c>
-      <c r="F9" s="5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75">
+    </row>
+    <row r="10" spans="1:2" ht="15.75">
       <c r="A10" s="3">
         <v>1080077</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5">
-        <v>16</v>
-      </c>
-      <c r="E10" s="5">
-        <v>32</v>
-      </c>
-      <c r="F10" s="5">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75">
+    </row>
+    <row r="11" spans="1:2" ht="15.75">
       <c r="A11" s="3">
         <v>1097085</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5">
-        <v>6</v>
-      </c>
-      <c r="E11" s="5">
-        <v>12</v>
-      </c>
-      <c r="F11" s="5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75">
+    </row>
+    <row r="12" spans="1:2" ht="15.75">
       <c r="A12" s="3">
         <v>1134845</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="5">
-        <v>12</v>
-      </c>
-      <c r="D12" s="5">
-        <v>24</v>
-      </c>
-      <c r="E12" s="5">
-        <v>36</v>
-      </c>
-      <c r="F12" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75">
+    </row>
+    <row r="13" spans="1:2" ht="15.75">
       <c r="A13" s="3">
         <v>1097067</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="5">
-        <v>15</v>
-      </c>
-      <c r="D13" s="5">
-        <v>30</v>
-      </c>
-      <c r="E13" s="5">
-        <v>45</v>
-      </c>
-      <c r="F13" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75">
+    </row>
+    <row r="14" spans="1:2" ht="15.75">
       <c r="A14" s="3">
         <v>1099659</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="5">
-        <v>15</v>
-      </c>
-      <c r="D14" s="5">
-        <v>30</v>
-      </c>
-      <c r="E14" s="5">
-        <v>45</v>
-      </c>
-      <c r="F14" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75">
+    </row>
+    <row r="15" spans="1:2" ht="15.75">
       <c r="A15" s="3">
         <v>1080073</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="5">
-        <v>12</v>
-      </c>
-      <c r="D15" s="5">
-        <v>24</v>
-      </c>
-      <c r="E15" s="5">
-        <v>36</v>
-      </c>
-      <c r="F15" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75">
+    </row>
+    <row r="16" spans="1:2" ht="15.75">
       <c r="A16" s="3">
         <v>1097074</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="5">
-        <v>12</v>
-      </c>
-      <c r="D16" s="5">
-        <v>24</v>
-      </c>
-      <c r="E16" s="5">
-        <v>36</v>
-      </c>
-      <c r="F16" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75">
+    </row>
+    <row r="17" spans="1:2" ht="15.75">
       <c r="A17" s="3">
         <v>1097082</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="5">
-        <v>12</v>
-      </c>
-      <c r="D17" s="5">
-        <v>24</v>
-      </c>
-      <c r="E17" s="5">
-        <v>36</v>
-      </c>
-      <c r="F17" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75">
+    </row>
+    <row r="18" spans="1:2" ht="15.75">
       <c r="A18" s="3">
         <v>1151765</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="5">
-        <v>12</v>
-      </c>
-      <c r="D18" s="5">
-        <v>24</v>
-      </c>
-      <c r="E18" s="5">
-        <v>36</v>
-      </c>
-      <c r="F18" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75">
+    </row>
+    <row r="19" spans="1:2" ht="15.75">
       <c r="A19" s="3">
         <v>1081854</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="5">
-        <v>8</v>
-      </c>
-      <c r="D19" s="5">
-        <v>16</v>
-      </c>
-      <c r="E19" s="5">
-        <v>32</v>
-      </c>
-      <c r="F19" s="5">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75">
+    </row>
+    <row r="20" spans="1:2" ht="15.75">
       <c r="A20" s="3">
         <v>1118534</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="5">
-        <v>3</v>
-      </c>
-      <c r="D20" s="5">
-        <v>6</v>
-      </c>
-      <c r="E20" s="5">
-        <v>12</v>
-      </c>
-      <c r="F20" s="5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75">
+    </row>
+    <row r="21" spans="1:2" ht="15.75">
       <c r="A21" s="3">
         <v>1134669</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="5">
-        <v>12</v>
-      </c>
-      <c r="D21" s="5">
-        <v>24</v>
-      </c>
-      <c r="E21" s="5">
-        <v>36</v>
-      </c>
-      <c r="F21" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75">
+    </row>
+    <row r="22" spans="1:2" ht="15.75">
       <c r="A22" s="3">
         <v>1136712</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="5">
-        <v>15</v>
-      </c>
-      <c r="D22" s="5">
-        <v>30</v>
-      </c>
-      <c r="E22" s="5">
-        <v>45</v>
-      </c>
-      <c r="F22" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75">
+    </row>
+    <row r="23" spans="1:2" ht="15.75">
       <c r="A23" s="3">
         <v>1134848</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="5">
-        <v>15</v>
-      </c>
-      <c r="D23" s="5">
-        <v>30</v>
-      </c>
-      <c r="E23" s="5">
-        <v>45</v>
-      </c>
-      <c r="F23" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75">
+    </row>
+    <row r="24" spans="1:2" ht="15.75">
       <c r="A24" s="3">
         <v>1097061</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="5">
-        <v>12</v>
-      </c>
-      <c r="D24" s="5">
-        <v>24</v>
-      </c>
-      <c r="E24" s="5">
-        <v>36</v>
-      </c>
-      <c r="F24" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75">
+    </row>
+    <row r="25" spans="1:2" ht="15.75">
       <c r="A25" s="3">
         <v>1097081</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="5">
-        <v>12</v>
-      </c>
-      <c r="D25" s="5">
-        <v>24</v>
-      </c>
-      <c r="E25" s="5">
-        <v>36</v>
-      </c>
-      <c r="F25" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75">
+    </row>
+    <row r="26" spans="1:2" ht="15.75">
       <c r="A26" s="3">
         <v>1122507</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="5">
-        <v>12</v>
-      </c>
-      <c r="D26" s="5">
-        <v>24</v>
-      </c>
-      <c r="E26" s="5">
-        <v>36</v>
-      </c>
-      <c r="F26" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75">
+    </row>
+    <row r="27" spans="1:2" ht="15.75">
       <c r="A27" s="3">
         <v>1099654</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="5">
-        <v>12</v>
-      </c>
-      <c r="D27" s="5">
-        <v>24</v>
-      </c>
-      <c r="E27" s="5">
-        <v>36</v>
-      </c>
-      <c r="F27" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75">
+    </row>
+    <row r="28" spans="1:2" ht="15.75">
       <c r="A28" s="3">
         <v>1102151</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="5">
-        <v>10</v>
-      </c>
-      <c r="D28" s="5">
-        <v>20</v>
-      </c>
-      <c r="E28" s="5">
-        <v>30</v>
-      </c>
-      <c r="F28" s="5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75">
+    </row>
+    <row r="29" spans="1:2" ht="15.75">
       <c r="A29" s="3">
         <v>1099662</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="5">
-        <v>8</v>
-      </c>
-      <c r="D29" s="5">
-        <v>16</v>
-      </c>
-      <c r="E29" s="5">
-        <v>32</v>
-      </c>
-      <c r="F29" s="5">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75">
+    </row>
+    <row r="30" spans="1:2" ht="15.75">
       <c r="A30" s="3">
         <v>1134843</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="5">
-        <v>3</v>
-      </c>
-      <c r="D30" s="5">
-        <v>6</v>
-      </c>
-      <c r="E30" s="5">
-        <v>12</v>
-      </c>
-      <c r="F30" s="5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75">
+    </row>
+    <row r="31" spans="1:2" ht="15.75">
       <c r="A31" s="3">
         <v>1080083</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="5">
-        <v>12</v>
-      </c>
-      <c r="D31" s="5">
-        <v>24</v>
-      </c>
-      <c r="E31" s="5">
-        <v>36</v>
-      </c>
-      <c r="F31" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75">
+    </row>
+    <row r="32" spans="1:2" ht="15.75">
       <c r="A32" s="3">
         <v>1152107</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="5">
-        <v>15</v>
-      </c>
-      <c r="D32" s="5">
-        <v>30</v>
-      </c>
-      <c r="E32" s="5">
-        <v>45</v>
-      </c>
-      <c r="F32" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75">
-      <c r="A33" s="3">
+    </row>
+    <row r="33" spans="1:2" ht="15.75">
+      <c r="A33" s="5">
         <v>1134668</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="5">
-        <v>15</v>
-      </c>
-      <c r="D33" s="5">
-        <v>30</v>
-      </c>
-      <c r="E33" s="5">
-        <v>45</v>
-      </c>
-      <c r="F33" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75">
+    </row>
+    <row r="34" spans="1:2" ht="15.75">
       <c r="A34" s="3">
         <v>1097072</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C34" s="5">
-        <v>12</v>
-      </c>
-      <c r="D34" s="5">
-        <v>24</v>
-      </c>
-      <c r="E34" s="5">
-        <v>36</v>
-      </c>
-      <c r="F34" s="5">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5E86BA-4545-4091-B845-A9E9CE6DCE14}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionando mensagens de alerta para QUANTIDADE e PRODUTOS
</commit_message>
<xml_diff>
--- a/mercadoria.xlsx
+++ b/mercadoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos_Phayton\Primeiro_Projeto_Pedidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EF2FA5-9422-499D-BEE6-BD93B17710ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA838A9-261E-41E8-B0AD-AE0F3FBE5348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DAC61F51-090E-4E48-8FA2-8D704C875542}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>cod_produto</t>
   </si>
@@ -44,110 +44,245 @@
     <t>desc_produto</t>
   </si>
   <si>
-    <t>PLANTA SUCULENTA PT 06</t>
-  </si>
-  <si>
-    <t>PLANTA CACTUS MINI P06</t>
-  </si>
-  <si>
-    <t>FLOR KALANCHOE P11</t>
-  </si>
-  <si>
-    <t>PLANTA ERVAS AROMAT PT 11</t>
-  </si>
-  <si>
-    <t>FLOR VIOLETA P11</t>
-  </si>
-  <si>
-    <t>FLOR MUDA CRISANTEMO PT11</t>
-  </si>
-  <si>
-    <t>PLANTA KALANCHOE T DA MONICA P06</t>
-  </si>
-  <si>
-    <t>FLOR ORQUIDEA PHALAENOPSIS P12</t>
-  </si>
-  <si>
-    <t>PLANTA PIMENTA P14</t>
-  </si>
-  <si>
-    <t>PLANTA SAMAMBAIA AMERICANA C21</t>
-  </si>
-  <si>
-    <t>PLANTA CACTUS VARIADO P11</t>
-  </si>
-  <si>
-    <t>PLANTA SUCULENTA PT11</t>
-  </si>
-  <si>
-    <t>FLOR ORQUIDEA DENPHALAEN P15</t>
-  </si>
-  <si>
-    <t>PLANTA PEPEROMIA C21</t>
-  </si>
-  <si>
-    <t>FLOR AZALEIA PT 14</t>
-  </si>
-  <si>
-    <t>PLANTA ARECA BAMBU PT 11</t>
-  </si>
-  <si>
-    <t>PLANTA LIRIO DA PAZ PT15</t>
-  </si>
-  <si>
-    <t>FLOR GIRASSOL P15</t>
-  </si>
-  <si>
-    <t>FLOR POINSETIA VERMELHA P14</t>
-  </si>
-  <si>
-    <t>PLANTA SUCULENTA PAPEL KRAFT</t>
-  </si>
-  <si>
-    <t>FLOR ROSA DO DESERTO P11</t>
-  </si>
-  <si>
-    <t>PLANTA SUCULENTAS C13</t>
-  </si>
-  <si>
-    <t>FLOR CRISANTEMO PT 13</t>
-  </si>
-  <si>
-    <t>PLANTA BONSAI JOVEM</t>
-  </si>
-  <si>
-    <t>PLANTA TUIA STRICKITA PT14</t>
-  </si>
-  <si>
-    <t>PLANTA AVENCA VARIADA P14</t>
-  </si>
-  <si>
-    <t>PLANTA TUIA HOLANDESA P14</t>
-  </si>
-  <si>
-    <t>PLANTA JIBOIA VERDE C21</t>
-  </si>
-  <si>
-    <t>PLANTA SUCULENTA C13 PENDENT</t>
-  </si>
-  <si>
-    <t>PLANTA ZAMIOCULCAS P17</t>
-  </si>
-  <si>
-    <t>PLANTA BROMELIA VARIADO P14</t>
-  </si>
-  <si>
-    <t>PLANTA ORQUIDEA PHALAENOPSI MIX P15</t>
-  </si>
-  <si>
-    <t>FLOR LIRIOS VARIADOS PT 15</t>
+    <t>AMARILIS PT14</t>
+  </si>
+  <si>
+    <t>ANTHURIUM VAR PT12</t>
+  </si>
+  <si>
+    <t>ANTHURIUM VAR PT15</t>
+  </si>
+  <si>
+    <t>ARECA BAMBU PT11</t>
+  </si>
+  <si>
+    <t>AVENCA PT14</t>
+  </si>
+  <si>
+    <t>AZALEIA PT14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEGONIA PT11  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEGONIA PT15 </t>
+  </si>
+  <si>
+    <t>BONSAI FRUTA  CX PLASTICA</t>
+  </si>
+  <si>
+    <t>BONSAI JOVEM</t>
+  </si>
+  <si>
+    <t>BROMELIA PT12</t>
+  </si>
+  <si>
+    <t>BROMELIA PT14</t>
+  </si>
+  <si>
+    <t>CACTUS MINI PT06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CACTUS PT11 MANDACARU </t>
+  </si>
+  <si>
+    <t>CALANDIVA  PT6 - (dobrado)</t>
+  </si>
+  <si>
+    <t>CALANDIVA PT11 - (dobrado)</t>
+  </si>
+  <si>
+    <t>CALANDIVA PT15 - (dobrado)</t>
+  </si>
+  <si>
+    <t>CASCA DE PINUS ( ALL GARDEN )</t>
+  </si>
+  <si>
+    <t>CELOSIA PT14</t>
+  </si>
+  <si>
+    <t>COQUETEL 7 ERVAS C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRISANTEMO PT11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRISANTEMO PT13  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURCUMA P15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYCLAMEN P14 </t>
+  </si>
+  <si>
+    <t>DIEFENBAQUIA P15</t>
+  </si>
+  <si>
+    <t>ECHEVERIA C21</t>
+  </si>
+  <si>
+    <t>ERVAS AROMATICAS PT11</t>
+  </si>
+  <si>
+    <t>EUONYMUS AUREUS PT15</t>
+  </si>
+  <si>
+    <t>FITONIA C13 MINI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GERBERA PT14  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIRASSOL PT11  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIRASSOL PT15  </t>
+  </si>
+  <si>
+    <t>HEDERA VARIEGATA C21</t>
+  </si>
+  <si>
+    <t>HIDROCULTURA PT06</t>
+  </si>
+  <si>
+    <t>HORTENSIA PT15</t>
+  </si>
+  <si>
+    <t>HUMUS ALL GARDEN</t>
+  </si>
+  <si>
+    <t>JIBOIA VERDE C21</t>
+  </si>
+  <si>
+    <t>LIRIO DA PAZ PT15</t>
+  </si>
+  <si>
+    <t>LIRIO VARIADO PT13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIRIO VARIADO PT15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LISIANTHUS JULIETTE PT12      </t>
+  </si>
+  <si>
+    <t>ORQ CYMBIDIUM PT18</t>
+  </si>
+  <si>
+    <t>ORQ DENDROBIUM NOBILY PT15</t>
+  </si>
+  <si>
+    <t>MAÇO DE PALMAS</t>
+  </si>
+  <si>
+    <t>MAÇO DE ROSAS COLORIDAS</t>
+  </si>
+  <si>
+    <t>ORQ DENPHALEN PT13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORQ PHALAENOPSIS  PT12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORQ PHALAENOPSIS  PT15 </t>
+  </si>
+  <si>
+    <t>ORQ VANDA COM VIDRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORQUIDEA ONCIDIUM POTE 15 </t>
+  </si>
+  <si>
+    <t>ORQ PHALAENOPSIS PT09</t>
+  </si>
+  <si>
+    <t>PEPERONIA C13</t>
+  </si>
+  <si>
+    <t>PALMEIRA RAPHIA PT17</t>
+  </si>
+  <si>
+    <t>PIMENTA  PT11</t>
+  </si>
+  <si>
+    <t>PEPERONIA SCANDES C21</t>
+  </si>
+  <si>
+    <t>POINSETTIA PT11</t>
+  </si>
+  <si>
+    <t>POINSETTIA PT14</t>
+  </si>
+  <si>
+    <t>PRIMULA PT 14</t>
+  </si>
+  <si>
+    <t>RENDA PORTUGUESA C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIMENTA PT 14 </t>
+  </si>
+  <si>
+    <t>ROSA DO DESERTO PT11</t>
+  </si>
+  <si>
+    <t>SAMAMBAIA HAVAIANA  C13</t>
+  </si>
+  <si>
+    <t>SUCULENTA PT06</t>
+  </si>
+  <si>
+    <t>ROSEIRA MINI PT13</t>
+  </si>
+  <si>
+    <t>SAMAMABAIA AMERICANA C21</t>
+  </si>
+  <si>
+    <t>SUCULENTA PT09 KRAFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUCULENTA PT11 </t>
+  </si>
+  <si>
+    <t>SUCULENTAS C21 PENDENTE</t>
+  </si>
+  <si>
+    <t>TERRA VEGETAL ALL GARDEN 2Kg</t>
+  </si>
+  <si>
+    <t>TERRARIO</t>
+  </si>
+  <si>
+    <t>TUIA HOLANDESA PT09</t>
+  </si>
+  <si>
+    <t>TUIA HOLANDESA PT20</t>
+  </si>
+  <si>
+    <t>TUIA STRICKTA PT20</t>
+  </si>
+  <si>
+    <t>TUIA STRICKTA PT24</t>
+  </si>
+  <si>
+    <t>TULIPA PT12 DECORADO MIX</t>
+  </si>
+  <si>
+    <t>SUCULENTAS C13 KRAFT</t>
+  </si>
+  <si>
+    <t>VIOLETA PT11</t>
+  </si>
+  <si>
+    <t>ZAMIOCULCA PT17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,14 +302,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,20 +316,8 @@
         <bgColor rgb="FFAFABAB"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2F0D9"/>
-        <bgColor rgb="FFE2F0D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFE2F0D9"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -221,27 +338,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -249,17 +351,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -576,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9DE960-2683-4898-8AD4-BC5936F3A2B4}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,271 +689,634 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75">
+    <row r="2" spans="1:2">
       <c r="A2" s="3">
-        <v>1097064</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75">
+    <row r="3" spans="1:2">
       <c r="A3" s="3">
-        <v>1099663</v>
-      </c>
-      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75">
+    <row r="4" spans="1:2">
       <c r="A4" s="3">
-        <v>1080071</v>
-      </c>
-      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
+    <row r="5" spans="1:2">
       <c r="A5" s="3">
-        <v>1097068</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75">
+    <row r="6" spans="1:2">
       <c r="A6" s="3">
-        <v>1080082</v>
-      </c>
-      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2">
       <c r="A7" s="3">
-        <v>1159663</v>
-      </c>
-      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75">
+    <row r="8" spans="1:2">
       <c r="A8" s="3">
-        <v>1129914</v>
-      </c>
-      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75">
-      <c r="A9" s="5">
-        <v>1080076</v>
-      </c>
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75">
+    <row r="10" spans="1:2">
       <c r="A10" s="3">
-        <v>1080077</v>
-      </c>
-      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75">
+    <row r="11" spans="1:2">
       <c r="A11" s="3">
-        <v>1097085</v>
-      </c>
-      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75">
+    <row r="12" spans="1:2">
       <c r="A12" s="3">
-        <v>1134845</v>
-      </c>
-      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75">
+    <row r="13" spans="1:2">
       <c r="A13" s="3">
-        <v>1097067</v>
-      </c>
-      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75">
+    <row r="14" spans="1:2">
       <c r="A14" s="3">
-        <v>1099659</v>
-      </c>
-      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75">
+    <row r="15" spans="1:2">
       <c r="A15" s="3">
-        <v>1080073</v>
-      </c>
-      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75">
+    <row r="16" spans="1:2">
       <c r="A16" s="3">
-        <v>1097074</v>
-      </c>
-      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75">
+    <row r="17" spans="1:2">
       <c r="A17" s="3">
-        <v>1097082</v>
-      </c>
-      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75">
+    <row r="18" spans="1:2">
       <c r="A18" s="3">
-        <v>1151765</v>
-      </c>
-      <c r="B18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75">
+    <row r="19" spans="1:2">
       <c r="A19" s="3">
-        <v>1081854</v>
-      </c>
-      <c r="B19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75">
+    <row r="20" spans="1:2">
       <c r="A20" s="3">
-        <v>1118534</v>
-      </c>
-      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75">
+    <row r="21" spans="1:2">
       <c r="A21" s="3">
-        <v>1134669</v>
-      </c>
-      <c r="B21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75">
+    <row r="22" spans="1:2">
       <c r="A22" s="3">
-        <v>1136712</v>
-      </c>
-      <c r="B22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75">
+    <row r="23" spans="1:2">
       <c r="A23" s="3">
-        <v>1134848</v>
-      </c>
-      <c r="B23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75">
+    <row r="24" spans="1:2">
       <c r="A24" s="3">
-        <v>1097061</v>
-      </c>
-      <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75">
+    <row r="25" spans="1:2">
       <c r="A25" s="3">
-        <v>1097081</v>
-      </c>
-      <c r="B25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75">
+    <row r="26" spans="1:2">
       <c r="A26" s="3">
-        <v>1122507</v>
-      </c>
-      <c r="B26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75">
+    <row r="27" spans="1:2">
       <c r="A27" s="3">
-        <v>1099654</v>
-      </c>
-      <c r="B27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75">
+    <row r="28" spans="1:2">
       <c r="A28" s="3">
-        <v>1102151</v>
-      </c>
-      <c r="B28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75">
+    <row r="29" spans="1:2">
       <c r="A29" s="3">
-        <v>1099662</v>
-      </c>
-      <c r="B29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75">
+    <row r="30" spans="1:2">
       <c r="A30" s="3">
-        <v>1134843</v>
-      </c>
-      <c r="B30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75">
+    <row r="31" spans="1:2">
       <c r="A31" s="3">
-        <v>1080083</v>
-      </c>
-      <c r="B31" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75">
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="3">
-        <v>1152107</v>
-      </c>
-      <c r="B32" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75">
-      <c r="A33" s="5">
-        <v>1134668</v>
-      </c>
-      <c r="B33" s="6" t="s">
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="3">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75">
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="3">
-        <v>1097072</v>
-      </c>
-      <c r="B34" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="3">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="3">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="3">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="3">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="3">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="3">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="3">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="3">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="3">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="3">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="3">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="3">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="3">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="3">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="3">
+        <v>54</v>
+      </c>
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="3">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="3">
+        <v>53</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="3">
+        <v>56</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="3">
+        <v>55</v>
+      </c>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="3">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="3">
+        <v>57</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="3">
+        <v>65</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="3">
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="3">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="3">
+        <v>61</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="3">
+        <v>62</v>
+      </c>
+      <c r="B61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="3">
+        <v>66</v>
+      </c>
+      <c r="B62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="3">
+        <v>69</v>
+      </c>
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="3">
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="3">
+        <v>67</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="3">
+        <v>68</v>
+      </c>
+      <c r="B66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="3">
+        <v>71</v>
+      </c>
+      <c r="B67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="3">
+        <v>72</v>
+      </c>
+      <c r="B68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="3">
+        <v>83</v>
+      </c>
+      <c r="B69" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="3">
+        <v>73</v>
+      </c>
+      <c r="B70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="3">
+        <v>74</v>
+      </c>
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="3">
+        <v>75</v>
+      </c>
+      <c r="B72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="3">
+        <v>76</v>
+      </c>
+      <c r="B73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="3">
+        <v>78</v>
+      </c>
+      <c r="B74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="3">
+        <v>80</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="3">
+        <v>81</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="3">
+        <v>82</v>
+      </c>
+      <c r="B77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="3">
+        <v>85</v>
+      </c>
+      <c r="B78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="3">
+        <v>86</v>
+      </c>
+      <c r="B79" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B85">
+    <sortCondition ref="B66:B85"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>